<commit_message>
Summenformel bei Keyword_Search eingetragen
</commit_message>
<xml_diff>
--- a/Documentation/Keyword_Search.xlsx
+++ b/Documentation/Keyword_Search.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sven\Documents\GitHub\AR-Education\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16125" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -142,12 +147,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -164,18 +175,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -501,23 +521,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="74.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="74.83203125" customWidth="1"/>
+    <col min="2" max="2" width="74.125" customWidth="1"/>
+    <col min="3" max="3" width="27.875" customWidth="1"/>
+    <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
+    <col min="6" max="6" width="74.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -537,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -554,7 +574,7 @@
         <v>41747</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -571,7 +591,7 @@
         <v>41747</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -588,7 +608,7 @@
         <v>41747</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -608,7 +628,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -625,7 +645,7 @@
         <v>41747</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -642,7 +662,7 @@
         <v>41747</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -657,6 +677,12 @@
       </c>
       <c r="E8" s="2">
         <v>41747</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <f>SUM(D2:D8)</f>
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Queries (esp. Benefits)
</commit_message>
<xml_diff>
--- a/Documentation/Keyword_Search.xlsx
+++ b/Documentation/Keyword_Search.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16125" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>ScienceDirect</t>
-  </si>
-  <si>
-    <t>http://web.a.ebscohost.com/ehost/resultsadvanced?sid=1e1a4532-aae6-4a24-8b60-423951a57d0c%40sessionmgr4005&amp;vid=4&amp;hid=4212&amp;bquery=TI+%28%22Augmented+Reality%22+AND+%28%22University*%22+OR+%22College*%22+OR+%22School*%22+OR+%22Teach*%22+OR+%22Learn*%22+OR+%22Educat*%22%29%29+OR+AB+%28%22Augmented+Reality%22+AND+%28%22University*%22+OR+%22College*%22+OR+%22School*%22+OR+%22Teach*%22+OR+%22Learn*%22+OR+%22Educat*%22%29%29+OR+KW+%28%22Augmented+Reality%22+AND+%28%22University*%22+OR+%22College*%22+OR+%22School*%22+OR+%22Teach*%22+OR+%22Learn*%22+OR+%22Educat*%22%29%29&amp;bdata=JmRiPWE5aCZkYj1idGgmdHlwZT0xJnNpdGU9ZWhvc3QtbGl2ZQ%3d%3d</t>
   </si>
   <si>
     <t xml:space="preserve">( 
@@ -131,30 +128,6 @@
     <t>http://ieeexplore.ieee.org/search/searchresult.jsp?action=search&amp;sortType=&amp;rowsPerPage=&amp;matchBoolean=true&amp;searchField=Search_All&amp;queryText=((%0A%20(%0A%20%20%22Document%20Title%22:%20%22Augmented%20Reality%22%20OR%0A%20%20%22Abstract%22:%20%22Augmented%20Reality%22%20OR%20%0A%20%20%22Author%20Keywords%22:%20%22Augmented%20Reality%22%0A%20)%20AND%20%0A%20(%0A%20%20%22Document%20Title%22:%20%22School%22%20OR%20%0A%20%20%22Document%20Title%22:%20%22Learn*%22%20OR%20%0A%20%20%22Document%20Title%22:%20%22Teach*%22%20OR%20%0A%20%20%22Document%20Title%22:%20%22Education%22%20OR%20%0A%0A%20%20%22Abstract%22:%20%22School*%22%20OR%20%0A%20%20%22Abstract%22:%20%22Learn*%22%20OR%20%0A%20%20%22Abstract%22:%20%22Teach*%22%20OR%20%0A%20%20%22Abstract%22:%20%22Education%22%20OR%0A%0A%20%20%22Author%20Keywords%22:%20%22School%22%20OR%20%0A%20%20%22Author%20Keywords%22:%20%22Learning%22%20OR%20%0A%20%20%22Author%20Keywords%22:%20%22Teaching%22%20OR%20%0A%20%20%22Author%20Keywords%22:%20%22Education%22%20%0A%20)%20%0A))</t>
   </si>
   <si>
-    <t xml:space="preserve">( 
- (
-  title: "Augmented Reality" OR 
-  abstract: "Augmented Reality" OR 
-  subject: "Augmented Reality"
- )
- AND
- (
-  title: (
-   "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*") 
-  ) OR 
-  abstract: (
-   "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*") 
-  ) OR 
-  subject: ( 
-   "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*") 
-  ) 
- )
-) </t>
-  </si>
-  <si>
-    <t>Fehler mit Solr auf Seite von AISeL</t>
-  </si>
-  <si>
     <t>(
  (
   TI (  
@@ -182,40 +155,43 @@
 )</t>
   </si>
   <si>
-    <t>http://web.b.ebscohost.com/ehost/resultsadvanced?sid=07a54ffd-e3c5-4126-b0f9-8edd79208ade%40sessionmgr111&amp;vid=4&amp;hid=112&amp;bquery=((TI+(%22Augmented+Reality%22)+OR+AB+(%22Augmented+Reality%22)+OR+KW+(%22Augmented+Reality%22))+AND+(TI+(%22College*%22+OR+%22School*%22+OR+%22Teach*%22+OR+%22Learn*%22+OR+%22Educat*%22)+OR+AB+(%22College*%22+OR+%22School*%22+OR+%22Teach*%22+OR+%22Learn*%22+OR+%22Educat*%22)+OR+KW+(%22College*%22+OR+%22School*%22+OR+%22Teach*%22+OR+%22Learn*%22+OR+%22Educat*%22)))&amp;bdata=JmRiPWE5aCZkYj1idGgmdHlwZT0xJnNpdGU9ZWhvc3QtbGl2ZQ%3d%3d</t>
-  </si>
-  <si>
-    <t>(
- (
-  TI° (  
-   "Augmented Reality" 
-  ) OR
-  AB° (  
-   "Augmented Reality" 
-  ) OR
-  KW° (  
-   "Augmented Reality" 
-  )
- )
+    <t>Artikel insgesamt</t>
+  </si>
+  <si>
+    <t>http://search.proquest.com/results/1EE1D94F9BA42E4PQ/1/$5bqueryType$3dcommandline:OS$3b+sortType$3drelevance$3b+searchTerms$3d$5b$3cAND$7call:$28TI$28$22Augmented+Reality$22$29+OR+AB$28$22Augmented+Reality$22$29+OR+SU$28$22Augmented+Reality$22$29$29+AND+$28TI$28$22College*$22+OR+$22School*$22+OR+$22Teach*$22+OR+$22Learn*$22+OR+$22Educat*$22$29+OR+AB$28$22College*$22+OR+$22School*$22+OR+$22Teach*$22+OR+$22Learn*$22+OR+$22Educat*$22$29+OR+SU$28$22College*$22+OR+$22School*$22+OR+$22Teach*$22+OR+$22Learn*$22+OR+$22Educat*$22$29$29+AND+$28TI$28$22Benefi*$22+OR+$22Advantag*$22$29+OR+AB$28$22Benefi*$22+OR+$22Advantag*$22$29+OR+SU$28$22Benefi*$22+OR+$22Advantag*$22$29$29$3e$5d$3b+searchParameters$3d$7bNAVIGATORS$3dnavsummarynav,sourcetypenav,pubtitlenav,objecttypenav,languagenav$28filter$3d200$2f0$2f*$29,decadenav$28filter$3d110$2f0$2f*,sort$3dname$2fascending$29,yearnav$28filter$3d1100$2f0$2f*,sort$3dname$2fascending$29,yearmonthnav$28filter$3d120$2f0$2f*,sort$3dname$2fascending$29,monthnav$28sort$3dname$2fascending$29,daynav$28sort$3dname$2fascending$29,+RS$3dOP,+chunkSize$3d20,+instance$3dprod.academic,+ftblock$3d740842+1+199113+113+670831+670829+660845+199000+660843+199001+660840,+removeDuplicates$3dtrue$7d$3b+metaData$3d$7bUsageSearchMode$3dCommandLine,+dbselections$3dallAvailable,+SEARCH_ID_TIMESTAMP$3d1398524529400$7d$5d?accountid=10218</t>
+  </si>
+  <si>
+    <t>http://web.a.ebscohost.com/ehost/resultsadvanced?sid=fbdefb89-6f81-40e9-bcec-68c5b3a0f64c%40sessionmgr4004&amp;vid=14&amp;hid=4206</t>
+  </si>
+  <si>
+    <t>http://dl.acm.org/results.cfm?within=%28+%0D%0A+Title%3A+%22Augmented+Reality%22+OR+%0D%0A+Abstract%3A+%22Augmented+Reality%22+OR+%0D%0A+Keywords%3A+%22Augmented+Reality%22%0D%0A%29+%0D%0AAND++%0D%0A%28+%0D%0A+%28+%0D%0A++Title%3A+%22College*%22+OR+%0D%0A++Title%3A+%22School*%22+OR+%0D%0A++Title%3A+%22Teach*%22+OR+%0D%0A++Title%3A+%22Learn*%22+OR+%0D%0A++Title%3A+%22Educat*%22+%0D%0A+%29+%0D%0A+OR++%0D%0A+%28+%0D%0A++Abstract%3A+%22College*%22+OR+%0D%0A++Abstract%3A+%22School*%22+OR+%0D%0A++Abstract%3A+%22Teach*%22+OR+%0D%0A++Abstract%3A+%22Learn*%22+OR+%0D%0A++Abstract%3A+%22Educat*%22+%0D%0A+%29+%0D%0A+OR+%0D%0A+%28+%0D%0A++Keywords%3A+%22College*%22+OR+%0D%0A++Keywords%3A+%22School*%22+OR+%0D%0A++Keywords%3A+%22Teach*%22+OR+%0D%0A++Keywords%3A+%22Learn*%22+OR+%0D%0A++Keywords%3A+%22Educat*%22+%0D%0A+%29+%0D%0A%29%0D%0AAND%0D%0A%28%0D%0A%28+%0D%0A++Title%3A+%22Benefi*%22+OR+%0D%0A++Title%3A+%22Advantag*%22++%0D%0A+%29+%0D%0A+OR++%0D%0A+%28+%0D%0A++Abstract%3A+%22Benefi*%22+OR+%0D%0A++Abstract%3A+%22Advantag*%22+%0D%0A+%29+%0D%0A+OR+%0D%0A+%28+%0D%0A++Keywords%3A+%22Benefi*%22+OR+%0D%0A++Keywords%3A+%22Advantag*%22+%0D%0A+%29+%0D%0A%29+&amp;CFID=327269280&amp;CFTOKEN=59077846&amp;adv=1&amp;COLL=DL&amp;qrycnt=405427&amp;DL=ACM&amp;Go.x=48&amp;Go.y=17&amp;termzone=all&amp;allofem=&amp;anyofem=&amp;noneofem=&amp;peoplezone=Name&amp;people=&amp;peoplehow=and&amp;keyword=&amp;keywordhow=AND&amp;affil=&amp;affilhow=AND&amp;pubin=&amp;pubinhow=and&amp;pubby=&amp;pubbyhow=OR&amp;since_year=&amp;before_year=&amp;pubashow=OR&amp;sponsor=&amp;sponsorhow=AND&amp;confdate=&amp;confdatehow=OR&amp;confloc=&amp;conflochow=OR&amp;isbnhow=OR&amp;isbn=&amp;doi=&amp;ccs=&amp;subj=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( 
+ ( 
+  title:( "Augmented Reality" ) OR 
+  abstract:( "Augmented Reality" ) OR 
+  subject:( "Augmented Reality" ) 
+ ) 
  AND 
- (
-  TI° (  
-   "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*"
-  ) OR
-  AB° (  
-   "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*"
-  ) OR
-  KW° (  
-   "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*"
-  )
- )
-)</t>
-  </si>
-  <si>
-    <t>http://search.proquest.com/results/DB136F1464E34A5BPQ/1/$5bqueryType$3dbasic:OS$3b+sortType$3drelevance$3b+searchTerms$3d$5b$3cAND$7ccitationBodyTags:$28$28all$28TI$b0$29+$28all$28$22Augmented+Reality$22$29$29+OR+all$28AB$b0$29+$28all$28$22Augmented+Reality$22$29$29+OR+all$28KW$b0$29+$28all$28$22Augmented+Reality$22$29$29$29+AND+$28all$28TI$b0$29+$28all$28$22College*$22$29+OR+all$28$22School*$22$29+OR+all$28$22Teach*$22$29+OR+all$28$22Learn*$22$29+OR+all$28$22Educat*$22$29$29+OR+all$28AB$b0$29+$28all$28$22College*$22$29+OR+all$28$22School*$22$29+OR+all$28$22Teach*$22$29+OR+all$28$22Learn*$22$29+OR+all$28$22Educat*$22$29$29+OR+all$28KW$b0$29+$28all$28$22College*$22$29+OR+all$28$22School*$22$29+OR+all$28$22Teach*$22$29+OR+all$28$22Learn*$22$29+OR+all$28$22Educat*$22$29$29$29$29$3e$5d$3b+searchParameters$3d$7bNAVIGATORS$3dnavsummarynav,sourcetypenav,pubtitlenav,objecttypenav,languagenav$28filter$3d200$2f0$2f*$29,decadenav$28filter$3d110$2f0$2f*,sort$3dname$2fascending$29,yearnav$28filter$3d1100$2f0$2f*,sort$3dname$2fascending$29,yearmonthnav$28filter$3d120$2f0$2f*,sort$3dname$2fascending$29,monthnav$28sort$3dname$2fascending$29,daynav$28sort$3dname$2fascending$29,+RS$3dOP,+flags$3dPeerReview,+chunkSize$3d20,+instance$3dprod.academic,+ftblock$3d740842+1+199113+113+670831+670829+660845+199000+660843+199001+660840,+removeDuplicates$3dtrue$7d$3b+metaData$3d$7bUsageSearchMode$3dQuickSearch,+dbselections$3dallAvailable,+SEARCH_ID_TIMESTAMP$3d1397909992584$7d$5d?accountid=10218</t>
-  </si>
-  <si>
-    <t>Artikel insgesamt</t>
+ ( 
+  title:(
+   "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*" 
+  ) OR 
+  abstract:( 
+   "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*" 
+  ) OR 
+  subject:( 
+   "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*" 
+  ) 
+ ) 
+) </t>
+  </si>
+  <si>
+    <t>http://aisel.aisnet.org/do/search/?q=(%20%20%20(%20%20%20%20title%3A(%20%22Augmented%20Reality%22%20)%20OR%20%20%20%20abstract%3A(%20%22Augmented%20Reality%22%20)%20OR%20%20%20%20subject%3A(%20%22Augmented%20Reality%22%20)%20%20%20)%20%20%20AND%20%20%20(%20%20%20%20title%3A(%20%20%20%20%22College*%22%20OR%20%22School*%22%20OR%20%22Teach*%22%20OR%20%22Learn*%22%20OR%20%22Educat*%22%20%20%20%20)%20OR%20%20%20%20abstract%3A(%20%20%20%20%20%22College*%22%20OR%20%22School*%22%20OR%20%22Teach*%22%20OR%20%22Learn*%22%20OR%20%22Educat*%22%20%20%20%20)%20OR%20%20%20%20subject%3A(%20%20%20%20%20%22College*%22%20OR%20%22School*%22%20OR%20%22Teach*%22%20OR%20%22Learn*%22%20OR%20%22Educat*%22%20%20%20%20)%20%20%20)%20%20)%20&amp;start=0&amp;context=509156</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ( TI( "Augmented Reality" ) OR AB( "Augmented Reality" ) OR SU( "Augmented Reality" ) ) AND ( TI( "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*" ) OR AB( "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*" ) OR SU( "College*" OR "School*" OR "Teach*" OR "Learn*" OR "Educat*" ) ) </t>
   </si>
 </sst>
 </file>
@@ -272,11 +248,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
@@ -288,11 +275,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+  <cellStyles count="16">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -629,20 +627,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="74.125" customWidth="1"/>
-    <col min="3" max="3" width="27.875" customWidth="1"/>
+    <col min="2" max="2" width="74.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
-    <col min="6" max="6" width="74.875" customWidth="1"/>
-    <col min="8" max="8" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="74.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -663,89 +663,89 @@
       </c>
       <c r="G1" s="1">
         <f>SUM(D:D)</f>
-        <v>919</v>
+        <v>653</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="60">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2">
-        <v>41750</v>
+        <v>41755</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="393.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="375">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3">
-        <v>189</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2">
-        <v>41750</v>
+        <v>41755</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="409">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4">
-        <v>186</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2">
-        <v>41750</v>
+        <v>41755</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="285">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
-        <v>41750</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
+        <v>41755</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="362.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="345">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
       <c r="D6">
         <v>418</v>
@@ -754,15 +754,15 @@
         <v>41750</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="120">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="D7">
         <v>125</v>

</xml_diff>